<commit_message>
Added assignment 4 database_structure.pdf, modified code a week ago
</commit_message>
<xml_diff>
--- a/raw_data/weekly_survival.xlsx
+++ b/raw_data/weekly_survival.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmg31\Box\Katy\Research\Experiments\Pteronarcys_Sulfate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmg31\Box\Katy\Research\experiments\sulfate\pteronarcys\raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2567E50-F6DC-49F1-B2AA-C6B47BDF0C23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E717EF4-0F7E-4944-B571-98CBC84B0700}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="156" yWindow="36" windowWidth="17772" windowHeight="12360" xr2:uid="{D37ECF63-FB3D-4FC0-B42B-560851217BCC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D37ECF63-FB3D-4FC0-B42B-560851217BCC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -400,7 +400,7 @@
   <dimension ref="A1:AA37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="AA18" sqref="AA18"/>
+      <selection activeCell="AC7" sqref="AC7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -567,6 +567,9 @@
       <c r="Z2">
         <v>7</v>
       </c>
+      <c r="AA2">
+        <v>7</v>
+      </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3">
@@ -647,6 +650,9 @@
       <c r="Z3">
         <v>9</v>
       </c>
+      <c r="AA3">
+        <v>9</v>
+      </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4">
@@ -727,6 +733,9 @@
       <c r="Z4">
         <v>1</v>
       </c>
+      <c r="AA4">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5">
@@ -807,6 +816,9 @@
       <c r="Z5">
         <v>9</v>
       </c>
+      <c r="AA5">
+        <v>9</v>
+      </c>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6">
@@ -887,6 +899,9 @@
       <c r="Z6">
         <v>1</v>
       </c>
+      <c r="AA6">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A7">
@@ -965,6 +980,9 @@
         <v>4</v>
       </c>
       <c r="Z7">
+        <v>4</v>
+      </c>
+      <c r="AA7">
         <v>4</v>
       </c>
     </row>
@@ -1047,6 +1065,9 @@
       <c r="Z8">
         <v>4</v>
       </c>
+      <c r="AA8">
+        <v>4</v>
+      </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A9">
@@ -1127,6 +1148,9 @@
       <c r="Z9">
         <v>9</v>
       </c>
+      <c r="AA9">
+        <v>9</v>
+      </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A10">
@@ -1207,6 +1231,9 @@
       <c r="Z10">
         <v>10</v>
       </c>
+      <c r="AA10">
+        <v>10</v>
+      </c>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A11">
@@ -1287,6 +1314,9 @@
       <c r="Z11">
         <v>7</v>
       </c>
+      <c r="AA11">
+        <v>7</v>
+      </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A12">
@@ -1367,6 +1397,9 @@
       <c r="Z12">
         <v>9</v>
       </c>
+      <c r="AA12">
+        <v>9</v>
+      </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A13">
@@ -1447,6 +1480,9 @@
       <c r="Z13">
         <v>7</v>
       </c>
+      <c r="AA13">
+        <v>7</v>
+      </c>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A14">
@@ -1527,6 +1563,9 @@
       <c r="Z14">
         <v>9</v>
       </c>
+      <c r="AA14">
+        <v>9</v>
+      </c>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A15">
@@ -1607,6 +1646,9 @@
       <c r="Z15">
         <v>8</v>
       </c>
+      <c r="AA15">
+        <v>8</v>
+      </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A16">
@@ -1687,8 +1729,11 @@
       <c r="Z16">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>3</v>
       </c>
@@ -1767,8 +1812,11 @@
       <c r="Z17">
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>3</v>
       </c>
@@ -1847,8 +1895,11 @@
       <c r="Z18">
         <v>8</v>
       </c>
-    </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>3</v>
       </c>
@@ -1927,8 +1978,11 @@
       <c r="Z19">
         <v>9</v>
       </c>
-    </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA19">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>4</v>
       </c>
@@ -2007,8 +2061,11 @@
       <c r="Z20">
         <v>6</v>
       </c>
-    </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA20">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>4</v>
       </c>
@@ -2087,8 +2144,11 @@
       <c r="Z21">
         <v>7</v>
       </c>
-    </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>4</v>
       </c>
@@ -2167,8 +2227,11 @@
       <c r="Z22">
         <v>6</v>
       </c>
-    </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA22">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>4</v>
       </c>
@@ -2247,8 +2310,11 @@
       <c r="Z23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>4</v>
       </c>
@@ -2327,8 +2393,11 @@
       <c r="Z24">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>4</v>
       </c>
@@ -2407,8 +2476,11 @@
       <c r="Z25">
         <v>7</v>
       </c>
-    </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>5</v>
       </c>
@@ -2487,8 +2559,11 @@
       <c r="Z26">
         <v>7</v>
       </c>
-    </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA26">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>5</v>
       </c>
@@ -2567,8 +2642,11 @@
       <c r="Z27">
         <v>7</v>
       </c>
-    </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA27">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>5</v>
       </c>
@@ -2647,8 +2725,11 @@
       <c r="Z28">
         <v>3</v>
       </c>
-    </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>5</v>
       </c>
@@ -2727,8 +2808,11 @@
       <c r="Z29">
         <v>8</v>
       </c>
-    </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA29">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>5</v>
       </c>
@@ -2807,8 +2891,11 @@
       <c r="Z30">
         <v>5</v>
       </c>
-    </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>5</v>
       </c>
@@ -2887,8 +2974,11 @@
       <c r="Z31">
         <v>7</v>
       </c>
-    </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA31">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>6</v>
       </c>
@@ -2967,8 +3057,11 @@
       <c r="Z32">
         <v>6</v>
       </c>
-    </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA32">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>6</v>
       </c>
@@ -3047,8 +3140,11 @@
       <c r="Z33">
         <v>6</v>
       </c>
-    </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA33">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>6</v>
       </c>
@@ -3127,8 +3223,11 @@
       <c r="Z34">
         <v>9</v>
       </c>
-    </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA34">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>6</v>
       </c>
@@ -3207,8 +3306,11 @@
       <c r="Z35">
         <v>7</v>
       </c>
-    </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>6</v>
       </c>
@@ -3287,8 +3389,11 @@
       <c r="Z36">
         <v>8</v>
       </c>
-    </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="AA36">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>6</v>
       </c>
@@ -3365,6 +3470,9 @@
         <v>9</v>
       </c>
       <c r="Z37">
+        <v>9</v>
+      </c>
+      <c r="AA37">
         <v>9</v>
       </c>
     </row>

</xml_diff>